<commit_message>
main: add cassandra support without wiring into batch config
</commit_message>
<xml_diff>
--- a/benchmarks/2020-07-29 Benchmark Results.xlsx
+++ b/benchmarks/2020-07-29 Benchmark Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17320" yWindow="5600" windowWidth="27840" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="5700" yWindow="4860" windowWidth="29940" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BATCH" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t># Records</t>
   </si>
@@ -51,30 +51,40 @@
     <t>Chunk Size</t>
   </si>
   <si>
-    <t>Inestion Time (s)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> # Records </t>
   </si>
   <si>
     <t xml:space="preserve"> Records per file </t>
   </si>
   <si>
-    <t>CPU Utilization</t>
-  </si>
-  <si>
-    <t>Packets Sent / s</t>
+    <t>Bulk Save (s)</t>
+  </si>
+  <si>
+    <t>Diff (%)</t>
+  </si>
+  <si>
+    <t>Per Record Time</t>
+  </si>
+  <si>
+    <t>Bulk Save Time</t>
+  </si>
+  <si>
+    <t>1B Extrapolation Time</t>
+  </si>
+  <si>
+    <t>Per Record Time (s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,12 +121,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,7 +147,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,7 +167,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -149,26 +177,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="174" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -445,43 +488,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="157" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>100000000</v>
       </c>
@@ -489,13 +549,31 @@
         <v>5000000</v>
       </c>
       <c r="C2" s="5">
-        <v>100000</v>
-      </c>
-      <c r="D2" s="5">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>500000</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5">
+        <v>415</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="11">
+        <f>D2/86400</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="15">
+        <f>10*D2/86400</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <f>E2/86400</f>
+        <v>4.8032407407407407E-3</v>
+      </c>
+      <c r="J2" s="12">
+        <f>10*E2/86400</f>
+        <v>4.8032407407407406E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>100000000</v>
       </c>
@@ -508,8 +586,31 @@
       <c r="D3" s="6">
         <v>829</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="5">
+        <v>371</v>
+      </c>
+      <c r="F3" s="10">
+        <f>(D3-E3)/D3</f>
+        <v>0.55247285886610376</v>
+      </c>
+      <c r="G3" s="11">
+        <f>D3/86400</f>
+        <v>9.5949074074074079E-3</v>
+      </c>
+      <c r="H3" s="15">
+        <f>10*D3/86400</f>
+        <v>9.5949074074074076E-2</v>
+      </c>
+      <c r="I3" s="11">
+        <f>E3/86400</f>
+        <v>4.2939814814814811E-3</v>
+      </c>
+      <c r="J3" s="12">
+        <f>10*E3/86400</f>
+        <v>4.2939814814814813E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>100000000</v>
       </c>
@@ -517,13 +618,37 @@
         <v>5000000</v>
       </c>
       <c r="C4" s="5">
-        <v>50000</v>
-      </c>
-      <c r="D4" s="6">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>100000</v>
+      </c>
+      <c r="D4" s="5">
+        <v>811</v>
+      </c>
+      <c r="E4" s="7">
+        <v>348</v>
+      </c>
+      <c r="F4" s="10">
+        <f>(D4-E4)/D4</f>
+        <v>0.5709001233045623</v>
+      </c>
+      <c r="G4" s="11">
+        <f>D4/86400</f>
+        <v>9.3865740740740732E-3</v>
+      </c>
+      <c r="H4" s="15">
+        <f>10*D4/86400</f>
+        <v>9.3865740740740736E-2</v>
+      </c>
+      <c r="I4" s="11">
+        <f>E4/86400</f>
+        <v>4.0277777777777777E-3</v>
+      </c>
+      <c r="J4" s="12">
+        <f>10*E4/86400</f>
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>100000000</v>
       </c>
@@ -531,13 +656,36 @@
         <v>5000000</v>
       </c>
       <c r="C5" s="5">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="D5" s="6">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>755</v>
+      </c>
+      <c r="E5" s="5">
+        <v>392</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" ref="F5:F12" si="0">(D5-E5)/D5</f>
+        <v>0.48079470198675495</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" ref="G5:G12" si="1">D5/86400</f>
+        <v>8.7384259259259255E-3</v>
+      </c>
+      <c r="H5" s="15">
+        <f t="shared" ref="H5:H12" si="2">10*D5/86400</f>
+        <v>8.7384259259259259E-2</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" ref="I5:I12" si="3">E5/86400</f>
+        <v>4.5370370370370373E-3</v>
+      </c>
+      <c r="J5" s="12">
+        <f t="shared" ref="J5:J12" si="4">10*E5/86400</f>
+        <v>4.5370370370370373E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>100000000</v>
       </c>
@@ -545,13 +693,36 @@
         <v>5000000</v>
       </c>
       <c r="C6" s="5">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="D6" s="6">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>737</v>
+      </c>
+      <c r="E6" s="7">
+        <v>385</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="0"/>
+        <v>0.47761194029850745</v>
+      </c>
+      <c r="G6" s="11">
+        <f t="shared" si="1"/>
+        <v>8.5300925925925926E-3</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" si="2"/>
+        <v>8.5300925925925933E-2</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" si="3"/>
+        <v>4.4560185185185189E-3</v>
+      </c>
+      <c r="J6" s="12">
+        <f t="shared" si="4"/>
+        <v>4.4560185185185182E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>100000000</v>
       </c>
@@ -559,13 +730,36 @@
         <v>5000000</v>
       </c>
       <c r="C7" s="5">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="D7" s="6">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>717</v>
+      </c>
+      <c r="E7" s="7">
+        <v>370</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>0.48396094839609483</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="1"/>
+        <v>8.2986111111111108E-3</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="2"/>
+        <v>8.2986111111111108E-2</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="3"/>
+        <v>4.2824074074074075E-3</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="4"/>
+        <v>4.2824074074074077E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>100000000</v>
       </c>
@@ -573,41 +767,110 @@
         <v>5000000</v>
       </c>
       <c r="C8" s="5">
+        <v>2500</v>
+      </c>
+      <c r="D8" s="6">
+        <v>713</v>
+      </c>
+      <c r="E8" s="7">
+        <v>372</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.47826086956521741</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="1"/>
+        <v>8.2523148148148148E-3</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="2"/>
+        <v>8.2523148148148151E-2</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="3"/>
+        <v>4.3055555555555555E-3</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="4"/>
+        <v>4.3055555555555555E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>100000000</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5000000</v>
+      </c>
+      <c r="C9" s="5">
         <v>1000</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <v>715</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>100000000</v>
-      </c>
-      <c r="B9" s="7">
+      <c r="E9" s="7">
+        <v>371</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.48111888111888113</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="1"/>
+        <v>8.2754629629629636E-3</v>
+      </c>
+      <c r="H9" s="15">
+        <f t="shared" si="2"/>
+        <v>8.2754629629629636E-2</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="3"/>
+        <v>4.2939814814814811E-3</v>
+      </c>
+      <c r="J9" s="12">
+        <f t="shared" si="4"/>
+        <v>4.2939814814814813E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
+        <v>100000000</v>
+      </c>
+      <c r="B10" s="17">
         <v>5000000</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="17">
         <v>500</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D10" s="18">
         <v>683</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>100000000</v>
-      </c>
-      <c r="B10" s="5">
-        <v>5000000</v>
-      </c>
-      <c r="C10" s="5">
-        <v>250</v>
-      </c>
-      <c r="D10" s="6">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="7">
+        <v>384</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="0"/>
+        <v>0.4377745241581259</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="H10" s="15">
+        <f t="shared" si="2"/>
+        <v>7.9050925925925927E-2</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="3"/>
+        <v>4.4444444444444444E-3</v>
+      </c>
+      <c r="J10" s="12">
+        <f t="shared" si="4"/>
+        <v>4.4444444444444446E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>100000000</v>
       </c>
@@ -615,14 +878,81 @@
         <v>5000000</v>
       </c>
       <c r="C11" s="5">
+        <v>250</v>
+      </c>
+      <c r="D11" s="6">
+        <v>696</v>
+      </c>
+      <c r="E11" s="7">
+        <v>399</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="0"/>
+        <v>0.42672413793103448</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="1"/>
+        <v>8.0555555555555554E-3</v>
+      </c>
+      <c r="H11" s="15">
+        <f t="shared" si="2"/>
+        <v>8.0555555555555561E-2</v>
+      </c>
+      <c r="I11" s="11">
+        <f t="shared" si="3"/>
+        <v>4.6180555555555558E-3</v>
+      </c>
+      <c r="J11" s="12">
+        <f t="shared" si="4"/>
+        <v>4.6180555555555558E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>100000000</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5000000</v>
+      </c>
+      <c r="C12" s="5">
         <v>100</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="6">
         <v>748</v>
       </c>
+      <c r="E12" s="7">
+        <v>471</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.37032085561497324</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="1"/>
+        <v>8.6574074074074071E-3</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" si="2"/>
+        <v>8.6574074074074067E-2</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" si="3"/>
+        <v>5.4513888888888893E-3</v>
+      </c>
+      <c r="J12" s="12">
+        <f t="shared" si="4"/>
+        <v>5.451388888888889E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>